<commit_message>
Adiciona arquivos resultantes do NMS
</commit_message>
<xml_diff>
--- a/Acuracia Resultados.xlsx
+++ b/Acuracia Resultados.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="417" documentId="13_ncr:1_{6DEE54BE-0BF6-4428-B6D2-0F659F733EDC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{AEC28EEC-1A7D-482F-A3AD-217DD44D63B2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="857" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9390" yWindow="1305" windowWidth="19410" windowHeight="8670" tabRatio="857" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TesteRede2_Binaria_Base2" sheetId="5" r:id="rId1"/>
@@ -6650,7 +6650,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$A$9</c15:sqref>
@@ -6676,7 +6676,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$1:$D$1</c15:sqref>
@@ -6699,7 +6699,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$9:$D$9</c15:sqref>
@@ -6712,7 +6712,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-34B0-4AD8-BDEA-40D076F1D215}"/>
                   </c:ext>
@@ -6725,7 +6725,7 @@
                 <c:order val="11"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$A$13</c15:sqref>
@@ -6751,7 +6751,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$1:$D$1</c15:sqref>
@@ -6774,7 +6774,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$13:$D$13</c15:sqref>
@@ -6787,7 +6787,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-34B0-4AD8-BDEA-40D076F1D215}"/>
                   </c:ext>
@@ -6800,7 +6800,7 @@
                 <c:order val="15"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$A$17</c15:sqref>
@@ -6827,7 +6827,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$1:$D$1</c15:sqref>
@@ -6850,7 +6850,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$17:$D$17</c15:sqref>
@@ -6863,7 +6863,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000F-34B0-4AD8-BDEA-40D076F1D215}"/>
                   </c:ext>
@@ -6876,7 +6876,7 @@
                 <c:order val="19"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$A$21</c15:sqref>
@@ -6902,7 +6902,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$1:$D$1</c15:sqref>
@@ -6925,7 +6925,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$21:$D$21</c15:sqref>
@@ -6938,7 +6938,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000013-34B0-4AD8-BDEA-40D076F1D215}"/>
                   </c:ext>
@@ -6951,7 +6951,7 @@
                 <c:order val="23"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$A$25</c15:sqref>
@@ -6977,7 +6977,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$1:$D$1</c15:sqref>
@@ -7000,7 +7000,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$25:$D$25</c15:sqref>
@@ -7013,7 +7013,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000017-34B0-4AD8-BDEA-40D076F1D215}"/>
                   </c:ext>
@@ -7026,7 +7026,7 @@
                 <c:order val="27"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$A$29</c15:sqref>
@@ -7053,7 +7053,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$1:$D$1</c15:sqref>
@@ -7076,7 +7076,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$29:$D$29</c15:sqref>
@@ -7089,7 +7089,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000001B-34B0-4AD8-BDEA-40D076F1D215}"/>
                   </c:ext>
@@ -7102,7 +7102,7 @@
                 <c:order val="31"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$A$33</c15:sqref>
@@ -7128,7 +7128,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$1:$D$1</c15:sqref>
@@ -7151,7 +7151,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$33:$D$33</c15:sqref>
@@ -7164,7 +7164,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000001F-34B0-4AD8-BDEA-40D076F1D215}"/>
                   </c:ext>
@@ -7177,7 +7177,7 @@
                 <c:order val="35"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$A$37</c15:sqref>
@@ -7203,7 +7203,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$1:$D$1</c15:sqref>
@@ -7226,7 +7226,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$37:$D$37</c15:sqref>
@@ -7239,7 +7239,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000023-34B0-4AD8-BDEA-40D076F1D215}"/>
                   </c:ext>
@@ -7252,7 +7252,7 @@
                 <c:order val="39"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$A$41</c15:sqref>
@@ -7279,7 +7279,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$1:$D$1</c15:sqref>
@@ -7302,7 +7302,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$41:$D$41</c15:sqref>
@@ -7315,7 +7315,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000027-34B0-4AD8-BDEA-40D076F1D215}"/>
                   </c:ext>
@@ -7328,7 +7328,7 @@
                 <c:order val="43"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$A$45</c15:sqref>
@@ -7354,7 +7354,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$1:$D$1</c15:sqref>
@@ -7377,7 +7377,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$45:$D$45</c15:sqref>
@@ -7390,7 +7390,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000002B-34B0-4AD8-BDEA-40D076F1D215}"/>
                   </c:ext>
@@ -7403,7 +7403,7 @@
                 <c:order val="47"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$A$49</c15:sqref>
@@ -7429,7 +7429,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$1:$D$1</c15:sqref>
@@ -7452,7 +7452,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Todos!$B$49:$D$49</c15:sqref>
@@ -7465,7 +7465,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000002F-34B0-4AD8-BDEA-40D076F1D215}"/>
                   </c:ext>
@@ -11046,7 +11046,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11249,7 +11249,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -11257,7 +11258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBA174E-1D73-43E4-BF72-24FDBDF63650}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14:D14"/>
     </sheetView>
   </sheetViews>
@@ -11468,8 +11469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEEA0E6F-1056-46B3-8A45-AC10040EAAE9}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>